<commit_message>
Establishing correct order of first eleven
</commit_message>
<xml_diff>
--- a/data/xlsx/22.03.16.0944 Applied tool analysis.xlsx
+++ b/data/xlsx/22.03.16.0944 Applied tool analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaveBabbitt\Documents\GitHub\itm-analysis-reporting\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0727B0A0-FDE2-4467-9B2C-491BB806A97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B0B34D-FF12-4C6F-8F89-94D2DC4F2052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7560" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1623,17 +1623,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P693"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A624" sqref="A624"/>
+    <sheetView tabSelected="1" topLeftCell="A484" workbookViewId="0">
+      <selection activeCell="A503" sqref="A503"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="36.21875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
-    <col min="7" max="7" width="50.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" customWidth="1"/>
+    <col min="5" max="6" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>